<commit_message>
Updating Allwyn dataset with education and experience
</commit_message>
<xml_diff>
--- a/data/allwyn.xlsx
+++ b/data/allwyn.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fangxinzhang/Documents/2021 summer/DAEN 690/week 4/python/file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miche/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC1934F6-FD73-4549-9B76-3BB82ECC0648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51943AD7-6C98-CF4E-983C-0070DF1D2C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{BD944EB7-8F77-3E41-AB57-7E16FF3377D1}"/>
   </bookViews>
@@ -34,9 +34,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>IT Project Manager I</t>
+  </si>
+  <si>
+    <t>IT Project Manager III</t>
+  </si>
+  <si>
+    <t>Senior Computer Security Systems Specialist</t>
+  </si>
+  <si>
+    <t>Senior Security Analyst</t>
+  </si>
+  <si>
+    <t>Cloud Engineer</t>
+  </si>
+  <si>
+    <t>Senior Data Scientist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+User Experience (UX) Developer</t>
+  </si>
+  <si>
+    <t>Health IT Software Developer I</t>
+  </si>
+  <si>
+    <t>Health IT Software Developer III</t>
+  </si>
+  <si>
+    <t>Test Automation Engineer</t>
+  </si>
+  <si>
+    <t>target job category</t>
+  </si>
+  <si>
+    <t>target description</t>
   </si>
   <si>
     <r>
@@ -52,65 +86,44 @@
       </rPr>
       <t>actionable information in a timely manner necessary to obtain decision/guidance to facilitate project execution.</t>
     </r>
-  </si>
-  <si>
-    <t>IT Project Manager III</t>
-  </si>
-  <si>
-    <t>Manages projects and development teams executing in a range of methodologies including waterfall, agile, and lean; Ensures the project meets scope, schedule, and budget; Serves as the Scrum Master for Agile projects; liaison between business and technical team; performs risk management; ensures government receives actionable information in a timely manner necessary to obtain decision/guidance to facilitate project execution.</t>
-  </si>
-  <si>
-    <t>Senior Computer Security Systems Specialist</t>
-  </si>
-  <si>
-    <t>Analyzes and defines security requirements for Multilevel Security (MLS) issues. Designs, develops, engineers, and implements solutions to MLS requirements. Responsible for the implementation and development of the MLS. Gathers and organizes technical information about an organization’s mission goals and needs, existing security products, and ongoing programs in the MLS arena. Performs risk analyses, which also include risk assessment. Provides daily supervision and direction to staff.</t>
-  </si>
-  <si>
-    <t>Senior Security Analyst</t>
-  </si>
-  <si>
-    <t>Analyzes security measures for more than one IT functional area (e.g., data, systems, network and/or Web) across the enterprise. Develops, implements, communicates and provides training of security assessments, policies and procedures Tracks, monitors, and enforces security policies, reviews security violation reports and investigates possible security exceptions, and updates, maintains and documents security controls. Prepares reports on security matters to develop security risk analysis scenarios and response procedures. Evaluates and recommends products and/or procedures to enhance productivity and effectiveness.</t>
-  </si>
-  <si>
-    <t>Cloud Engineer</t>
-  </si>
-  <si>
-    <t>Experience with cloud services - including open source technology, software development, system engineering, scripting languages and multiple cloud provider environments. Additionally, Cloud engineers need to be familiar with one or more of the following: OpenStack, Amazon Web Services, Rackspace, Google Compute Engine, Microsoft Azure and Docker. Experience with APIs, orchestration, automation and DevOps are also important</t>
-  </si>
-  <si>
-    <t>Senior Data Scientist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Scientist will have necessary statistical modelling, mathematical, big data analytics and predictive modelling skills to build the required algorithms necessary to ask right questions and build objective visualizations and findings from it. Data Scientist will have knowledge of integrating multiple systems and datasets to provide new insights. Examples of required skillset: • Prior experience working as a data architect and managing information schema for large organizations • Experience with big data analytic tools such as Hadoop, Hive, MapReduce, SPLUNK, Elastic Search • Understanding and good working knowledge of SQL and NoSQL • Experience in machine learning, statistical modelling, and predictive analysis • Extensive experience with a statistical programming language.
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Minimum Education: A Bachelor’s Degree Minimum Experience: Five (5) years</t>
+    </r>
+  </si>
+  <si>
+    <t>Manages projects and development teams executing in a range of methodologies including waterfall, agile, and lean; Ensures the project meets scope, schedule, and budget; Serves as the Scrum Master for Agile projects; liaison between business and technical team; performs risk management; ensures government receives actionable information in a timely manner necessary to obtain decision/guidance to facilitate project execution. Minimum Education: A Bachelor’s Degree Minimum Experience: Ten (10) years</t>
+  </si>
+  <si>
+    <t>Analyzes and defines security requirements for Multilevel Security (MLS) issues. Designs, develops, engineers, and implements solutions to MLS requirements. Responsible for the implementation and development of the MLS. Gathers and organizes technical information about an organization’s mission goals and needs, existing security products, and ongoing programs in the MLS arena. Performs risk analyses, which also include risk assessment. Provides daily supervision and direction to staff. Minimum Education: A Bachelor’s Degree Minimum Experience: Eight (8) years</t>
+  </si>
+  <si>
+    <t>Analyzes security measures for more than one IT functional area (e.g., data, systems, network and/or Web) across the enterprise. Develops, implements, communicates and provides training of security assessments, policies and procedures Tracks, monitors, and enforces security policies, reviews security violation reports and investigates possible security exceptions, and updates, maintains and documents security controls. Prepares reports on security matters to develop security risk analysis scenarios and response procedures. Evaluates and recommends products and/or procedures to enhance productivity and effectiveness. Minimum Education: A Bachelor’s Degree Minimum Experience: Seven (7) years</t>
+  </si>
+  <si>
+    <t>Experience with cloud services - including open source technology, software development, system engineering, scripting languages and multiple cloud provider environments. Additionally, Cloud engineers need to be familiar with one or more of the following: OpenStack, Amazon Web Services, Rackspace, Google Compute Engine, Microsoft Azure and Docker. Experience with APIs, orchestration, automation and DevOps are also important. Minimum Education: A Bachelor’s Degree Minimum Experience: Seven (7) years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Scientist will have necessary statistical modelling, mathematical, big data analytics and predictive modelling skills to build the required algorithms necessary to ask right questions and build objective visualizations and findings from it. Data Scientist will have knowledge of integrating multiple systems and datasets to provide new insights. Examples of required skillset: • Prior experience working as a data architect and managing information schema for large organizations • Experience with big data analytic tools such as Hadoop, Hive, MapReduce, SPLUNK, Elastic Search • Understanding and good working knowledge of SQL and NoSQL • Experience in machine learning, statistical modelling, and predictive analysis • Extensive experience with a statistical programming language. Minimum Education: A Bachelor’s Degree Minimum Experience: Seven (7) years
 </t>
   </si>
   <si>
-    <t xml:space="preserve">
-User Experience (UX) Developer</t>
-  </si>
-  <si>
-    <t>Responsible for creating front-end design solutions for both web and mobile platforms. The role involves working closely with project manager, analyst, developers and testers to determine ideal design solution. Conduct usability testing to make sure design satisfies all project requirements. Required skillset: • Design mock-up templates using a combination of tools such as HTML, CSS, Photoshop and other standard industry design tools. • Develop responsive design in HTML5 and CSS3 for mobile compatibility • Experience with JavaScript • Experience designing graphics and UI for mobile development • Expertise in Adobe Creative Suite • Design custom logos and images • Understanding of up to date web standards and specifications • Experience with distributed source control systems such as git.</t>
-  </si>
-  <si>
-    <t>Health IT Software Developer I</t>
-  </si>
-  <si>
-    <t>Develop, modify, or update applications used by business units or infrastructure units. Lead, or play lead technical role in development teams' efforts to determine unit needs and business processes that are automated by the application. Participate in or review all of the steps in the software development life cycle to create and modify the software.</t>
-  </si>
-  <si>
-    <t>Health IT Software Developer III</t>
-  </si>
-  <si>
-    <t>Test Automation Engineer</t>
-  </si>
-  <si>
-    <t>The Test Automation Engineer is responsible for the analysis of project functional requirements as well as development of code in Java for automating test scenarios. The incumbent is responsible for the analysis of functional requirements, testing applications, developing test plans, test cases and test scripts, and evaluating test results to determine compliance with test plans and established business processes.</t>
-  </si>
-  <si>
-    <t>target job category</t>
-  </si>
-  <si>
-    <t>target description</t>
+    <t>Responsible for creating front-end design solutions for both web and mobile platforms. The role involves working closely with project manager, analyst, developers and testers to determine ideal design solution. Conduct usability testing to make sure design satisfies all project requirements. Required skillset: • Design mock-up templates using a combination of tools such as HTML, CSS, Photoshop and other standard industry design tools. • Develop responsive design in HTML5 and CSS3 for mobile compatibility • Experience with JavaScript • Experience designing graphics and UI for mobile development • Expertise in Adobe Creative Suite • Design custom logos and images • Understanding of up to date web standards and specifications • Experience with distributed source control systems such as git. Minimum Education: A Bachelor’s Degree Minimum Experience: Seven (7) years</t>
+  </si>
+  <si>
+    <t>Develop, modify, or update applications used by business units or infrastructure units. Lead, or play lead technical role in development teams' efforts to determine unit needs and business processes that are automated by the application. Participate in or review all of the steps in the software development life cycle to create and modify the software. Minimum Education: A Bachelor’s Degree Minimum Experience: Five (5) Years</t>
+  </si>
+  <si>
+    <t>Develop, modify, or update applications used by business units or infrastructure units. Lead, or play lead technical role in development teams' efforts to determine unit needs and business processes that are automated by the application. Participate in or review all of the steps in the software development life cycle to create and modify the software. Minimum Education: A Bachelor’s Degree Minimum Experience: Ten (10) Years</t>
+  </si>
+  <si>
+    <t>The Test Automation Engineer is responsible for the analysis of project functional requirements as well as development of code in Java for automating test scenarios. The incumbent is responsible for the analysis of functional requirements, testing applications, developing test plans, test cases and test scripts, and evaluating test results to determine compliance with test plans and established business processes. Minimum Education: A Bachelor’s Degree Minimum Experience: Five (5) years</t>
   </si>
 </sst>
 </file>
@@ -489,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E698E68-6A8D-D84B-8E99-D8D87E50555D}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,90 +514,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="204" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="136" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="187" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="170" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>